<commit_message>
#1189143 - changed the conference numbers to reflect the new format - with Michael Adams
</commit_message>
<xml_diff>
--- a/Raw/Excel Files/test/bigBook.xlsx
+++ b/Raw/Excel Files/test/bigBook.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\Court-Scheduler\Raw\Excel Files\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
   <si>
     <t>TEAM  LIST  AS  OF :</t>
   </si>
@@ -280,6 +285,24 @@
   </si>
   <si>
     <t>NO 1/14/14-1/15/14, NO 1/21/14-1/22/14, NO 2/11/14-2/12/14, NO 2/24/14-2/25/14</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>2c</t>
   </si>
 </sst>
 </file>
@@ -876,6 +899,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -923,7 +949,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -958,7 +984,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1169,26 +1195,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625"/>
-    <col min="4" max="4" width="8.7109375"/>
-    <col min="5" max="5" width="7.5703125"/>
-    <col min="6" max="6" width="7.140625"/>
-    <col min="7" max="7" width="5.85546875"/>
-    <col min="8" max="8" width="124.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875"/>
-    <col min="10" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="8.7109375"/>
+    <col min="2" max="2" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125"/>
+    <col min="5" max="5" width="7.54296875"/>
+    <col min="6" max="6" width="7.1796875"/>
+    <col min="7" max="7" width="5.81640625"/>
+    <col min="8" max="8" width="124.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.81640625"/>
+    <col min="10" max="11" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1223,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>26</v>
@@ -1237,12 +1261,12 @@
       <c r="S2" s="27"/>
       <c r="T2" s="27"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>101</v>
       </c>
-      <c r="B3" s="12">
-        <v>11</v>
+      <c r="B3" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>8</v>
@@ -1271,12 +1295,12 @@
       <c r="S3" s="36"/>
       <c r="T3" s="36"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>102</v>
       </c>
-      <c r="B4" s="12">
-        <v>11</v>
+      <c r="B4" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>11</v>
@@ -1307,12 +1331,12 @@
       <c r="S4" s="36"/>
       <c r="T4" s="36"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>103</v>
       </c>
-      <c r="B5" s="12">
-        <v>11</v>
+      <c r="B5" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>14</v>
@@ -1343,12 +1367,12 @@
       <c r="S5" s="36"/>
       <c r="T5" s="36"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>104</v>
       </c>
-      <c r="B6" s="12">
-        <v>11</v>
+      <c r="B6" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>16</v>
@@ -1379,12 +1403,12 @@
       <c r="S6" s="36"/>
       <c r="T6" s="36"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>105</v>
       </c>
-      <c r="B7" s="12">
-        <v>11</v>
+      <c r="B7" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>19</v>
@@ -1417,12 +1441,12 @@
       <c r="S7" s="36"/>
       <c r="T7" s="36"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>106</v>
       </c>
-      <c r="B8" s="12">
-        <v>11</v>
+      <c r="B8" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>22</v>
@@ -1453,12 +1477,12 @@
       <c r="S8" s="36"/>
       <c r="T8" s="36"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>107</v>
       </c>
-      <c r="B9" s="12">
-        <v>11</v>
+      <c r="B9" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>24</v>
@@ -1489,12 +1513,12 @@
       <c r="S9" s="36"/>
       <c r="T9" s="36"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="46">
         <v>141</v>
       </c>
-      <c r="B10" s="12">
-        <v>12</v>
+      <c r="B10" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="C10" s="48" t="s">
         <v>27</v>
@@ -1523,12 +1547,12 @@
       <c r="S10" s="36"/>
       <c r="T10" s="36"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="46">
         <v>142</v>
       </c>
-      <c r="B11" s="1">
-        <v>12</v>
+      <c r="B11" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C11" s="48" t="s">
         <v>28</v>
@@ -1561,12 +1585,12 @@
       <c r="S11" s="36"/>
       <c r="T11" s="36"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="46">
         <v>143</v>
       </c>
-      <c r="B12" s="1">
-        <v>12</v>
+      <c r="B12" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C12" s="48" t="s">
         <v>30</v>
@@ -1597,12 +1621,12 @@
       <c r="S12" s="36"/>
       <c r="T12" s="36"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="46">
         <v>145</v>
       </c>
-      <c r="B13" s="1">
-        <v>12</v>
+      <c r="B13" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C13" s="48" t="s">
         <v>31</v>
@@ -1633,12 +1657,12 @@
       <c r="S13" s="36"/>
       <c r="T13" s="36"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="46">
         <v>146</v>
       </c>
-      <c r="B14" s="1">
-        <v>12</v>
+      <c r="B14" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C14" s="48" t="s">
         <v>32</v>
@@ -1669,12 +1693,12 @@
       <c r="S14" s="36"/>
       <c r="T14" s="36"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="46">
         <v>151</v>
       </c>
-      <c r="B15" s="1">
-        <v>13</v>
+      <c r="B15" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C15" s="48" t="s">
         <v>33</v>
@@ -1705,12 +1729,12 @@
       <c r="S15" s="36"/>
       <c r="T15" s="36"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="46">
         <v>152</v>
       </c>
-      <c r="B16" s="1">
-        <v>13</v>
+      <c r="B16" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C16" s="48" t="s">
         <v>35</v>
@@ -1739,12 +1763,12 @@
       <c r="S16" s="36"/>
       <c r="T16" s="36"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="46">
         <v>153</v>
       </c>
-      <c r="B17" s="1">
-        <v>13</v>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C17" s="48" t="s">
         <v>36</v>
@@ -1773,12 +1797,12 @@
       <c r="S17" s="36"/>
       <c r="T17" s="36"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="46">
         <v>154</v>
       </c>
-      <c r="B18" s="1">
-        <v>13</v>
+      <c r="B18" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C18" s="48" t="s">
         <v>37</v>
@@ -1807,12 +1831,12 @@
       <c r="S18" s="36"/>
       <c r="T18" s="36"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="46">
         <v>155</v>
       </c>
-      <c r="B19" s="1">
-        <v>13</v>
+      <c r="B19" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C19" s="48" t="s">
         <v>38</v>
@@ -1841,12 +1865,12 @@
       <c r="S19" s="36"/>
       <c r="T19" s="36"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="46">
         <v>156</v>
       </c>
-      <c r="B20" s="1">
-        <v>13</v>
+      <c r="B20" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C20" s="48" t="s">
         <v>39</v>
@@ -1875,12 +1899,12 @@
       <c r="S20" s="36"/>
       <c r="T20" s="36"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="46">
         <v>208</v>
       </c>
-      <c r="B21" s="1">
-        <v>21</v>
+      <c r="B21" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C21" s="48" t="s">
         <v>40</v>
@@ -1911,12 +1935,12 @@
       <c r="S21" s="36"/>
       <c r="T21" s="36"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="46">
         <v>207</v>
       </c>
-      <c r="B22" s="1">
-        <v>21</v>
+      <c r="B22" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C22" s="48" t="s">
         <v>41</v>
@@ -1945,12 +1969,12 @@
       <c r="S22" s="36"/>
       <c r="T22" s="36"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="46">
         <v>2014</v>
       </c>
-      <c r="B23" s="1">
-        <v>21</v>
+      <c r="B23" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>42</v>
@@ -1983,12 +2007,12 @@
       <c r="S23" s="36"/>
       <c r="T23" s="36"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="46">
         <v>2015</v>
       </c>
-      <c r="B24" s="1">
-        <v>21</v>
+      <c r="B24" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C24" s="48" t="s">
         <v>44</v>
@@ -2017,12 +2041,12 @@
       <c r="S24" s="36"/>
       <c r="T24" s="36"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="46">
         <v>2016</v>
       </c>
-      <c r="B25" s="1">
-        <v>21</v>
+      <c r="B25" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C25" s="48" t="s">
         <v>45</v>
@@ -2051,12 +2075,12 @@
       <c r="S25" s="36"/>
       <c r="T25" s="36"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="46">
         <v>2013</v>
       </c>
-      <c r="B26" s="1">
-        <v>21</v>
+      <c r="B26" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C26" s="48" t="s">
         <v>46</v>
@@ -2087,12 +2111,12 @@
       <c r="S26" s="36"/>
       <c r="T26" s="36"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="46">
         <v>203</v>
       </c>
-      <c r="B27" s="1">
-        <v>21</v>
+      <c r="B27" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C27" s="48" t="s">
         <v>47</v>
@@ -2121,12 +2145,12 @@
       <c r="S27" s="36"/>
       <c r="T27" s="36"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="56">
         <v>2012</v>
       </c>
-      <c r="B28" s="1">
-        <v>21</v>
+      <c r="B28" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C28" s="48" t="s">
         <v>48</v>
@@ -2157,12 +2181,12 @@
       <c r="S28" s="36"/>
       <c r="T28" s="36"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="65">
         <v>206</v>
       </c>
-      <c r="B29" s="1">
-        <v>22</v>
+      <c r="B29" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C29" s="50" t="s">
         <v>49</v>
@@ -2193,12 +2217,12 @@
       <c r="S29" s="36"/>
       <c r="T29" s="36"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="46">
         <v>202</v>
       </c>
-      <c r="B30" s="1">
-        <v>22</v>
+      <c r="B30" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C30" s="48" t="s">
         <v>50</v>
@@ -2229,12 +2253,12 @@
       <c r="S30" s="36"/>
       <c r="T30" s="36"/>
     </row>
-    <row r="31" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A31" s="46">
         <v>2010</v>
       </c>
-      <c r="B31" s="1">
-        <v>22</v>
+      <c r="B31" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C31" s="48" t="s">
         <v>52</v>
@@ -2265,12 +2289,12 @@
       <c r="S31" s="36"/>
       <c r="T31" s="68"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="46">
         <v>205</v>
       </c>
-      <c r="B32" s="1">
-        <v>22</v>
+      <c r="B32" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C32" s="48" t="s">
         <v>53</v>
@@ -2301,12 +2325,12 @@
       <c r="S32" s="36"/>
       <c r="T32" s="36"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" s="46">
         <v>2011</v>
       </c>
-      <c r="B33" s="1">
-        <v>22</v>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C33" s="48" t="s">
         <v>55</v>
@@ -2337,12 +2361,12 @@
       <c r="S33" s="36"/>
       <c r="T33" s="36"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" s="46">
         <v>209</v>
       </c>
-      <c r="B34" s="1">
-        <v>22</v>
+      <c r="B34" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C34" s="48" t="s">
         <v>56</v>
@@ -2373,12 +2397,12 @@
       <c r="S34" s="36"/>
       <c r="T34" s="36"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" s="46">
         <v>204</v>
       </c>
-      <c r="B35" s="1">
-        <v>22</v>
+      <c r="B35" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C35" s="48" t="s">
         <v>57</v>
@@ -2407,12 +2431,12 @@
       <c r="S35" s="36"/>
       <c r="T35" s="75"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" s="46">
         <v>201</v>
       </c>
-      <c r="B36" s="1">
-        <v>22</v>
+      <c r="B36" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C36" s="48" t="s">
         <v>58</v>
@@ -2445,12 +2469,12 @@
       <c r="S36" s="36"/>
       <c r="T36" s="36"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="46">
         <v>221</v>
       </c>
-      <c r="B37" s="1">
-        <v>23</v>
+      <c r="B37" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C37" s="48" t="s">
         <v>60</v>
@@ -2483,12 +2507,12 @@
       <c r="S37" s="36"/>
       <c r="T37" s="36"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="46">
         <v>222</v>
       </c>
-      <c r="B38" s="1">
-        <v>23</v>
+      <c r="B38" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C38" s="48" t="s">
         <v>62</v>
@@ -2521,12 +2545,12 @@
       <c r="S38" s="36"/>
       <c r="T38" s="36"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" s="46">
         <v>223</v>
       </c>
-      <c r="B39" s="1">
-        <v>23</v>
+      <c r="B39" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C39" s="48" t="s">
         <v>64</v>
@@ -2557,12 +2581,12 @@
       <c r="S39" s="36"/>
       <c r="T39" s="36"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" s="46">
         <v>224</v>
       </c>
-      <c r="B40" s="1">
-        <v>23</v>
+      <c r="B40" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C40" s="48" t="s">
         <v>66</v>
@@ -2595,12 +2619,12 @@
       <c r="S40" s="36"/>
       <c r="T40" s="36"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" s="46">
         <v>225</v>
       </c>
-      <c r="B41" s="1">
-        <v>23</v>
+      <c r="B41" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C41" s="48" t="s">
         <v>68</v>
@@ -2631,12 +2655,12 @@
       <c r="S41" s="36"/>
       <c r="T41" s="36"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" s="65">
         <v>226</v>
       </c>
-      <c r="B42" s="1">
-        <v>23</v>
+      <c r="B42" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C42" s="48" t="s">
         <v>70</v>
@@ -2736,10 +2760,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2752,10 +2773,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>